<commit_message>
site accessible et avancees tableau audit
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="936" yWindow="624" windowWidth="23436" windowHeight="17376" tabRatio="500"/>
@@ -10,22 +10,12 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgajbA1sRpj4h647px0Becg4xhqcQ=="/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Catégorie</t>
   </si>
@@ -46,13 +36,178 @@
   </si>
   <si>
     <t>(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t>Taille police text centre white</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Contraste avec hover</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contraste assez important notamment pour les malvoyants on ne voit pas assez le changement de contraste et donc la possibilité d'interaction</t>
+  </si>
+  <si>
+    <t>La taille de police est petite c'est une difficulté pour les malvoyants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Côté local de l'agence Lyon </t>
+  </si>
+  <si>
+    <t>Le côté local revient dans le texte, mais on ne le retrouve pas au niveau des mots-clés on retrouve Paris, mais pas Lyon</t>
+  </si>
+  <si>
+    <t>quel est le problème ?</t>
+  </si>
+  <si>
+    <t>En quoi c'est un pb ?</t>
+  </si>
+  <si>
+    <t>Comment résoudre le pb ?</t>
+  </si>
+  <si>
+    <t>source d'information</t>
+  </si>
+  <si>
+    <t>hvk</t>
+  </si>
+  <si>
+    <t>pas d'utilisation de balise canonique</t>
+  </si>
+  <si>
+    <t>Pas de définition de la langue</t>
+  </si>
+  <si>
+    <t>Viewport fit cover?</t>
+  </si>
+  <si>
+    <t>dans les div bg white te dark, les class sont trop longues</t>
+  </si>
+  <si>
+    <t>Balise meta pas de titre pour les pages 1 et 2</t>
+  </si>
+  <si>
+    <t>Lien contact pas d'explication de la signification du lien</t>
+  </si>
+  <si>
+    <t>Bloc tc -white du mal à distinguer le texte duu fond…</t>
+  </si>
+  <si>
+    <t>Icones n'ont pas de aria label</t>
+  </si>
+  <si>
+    <t>Pas de description des icones</t>
+  </si>
+  <si>
+    <t>role = "img" aria-label="crayon" à rajouter dans la span illustration crayon par exemple</t>
+  </si>
+  <si>
+    <t>Absence de balise structurante</t>
+  </si>
+  <si>
+    <t>Les balises structurantes aident les robots à comprendre l'organisation du contenu et de ce fait améliorent le SEO</t>
+  </si>
+  <si>
+    <t>Il est préférable de définir une langue pour les robots de google</t>
+  </si>
+  <si>
+    <t>&lt;html lang="fr"&gt;</t>
+  </si>
+  <si>
+    <t>Titre de page non définis</t>
+  </si>
+  <si>
+    <t>Pas d'indexation des moteurs de recherche</t>
+  </si>
+  <si>
+    <t>Il faut indiquer via les balises meta name robots qu'on autorise indexation par les moteurs de recherche, sinon il peut y avaoir blocage au niveau des moteurs de recherche</t>
+  </si>
+  <si>
+    <t>Pas de balise canonique</t>
+  </si>
+  <si>
+    <t>Image pas décrite</t>
+  </si>
+  <si>
+    <t>Afin que les malvoyants ou non voyants aient accès à l'image, il faudrait rajouter une description des images</t>
+  </si>
+  <si>
+    <t>dans balise img mettre alt suivi de description de l'image"</t>
+  </si>
+  <si>
+    <t>Dans le html incorporer des balises structurantes de type header nav etc</t>
+  </si>
+  <si>
+    <t>wcag</t>
+  </si>
+  <si>
+    <t>Contraste des couleurs du bouton entre 1er et arrière plan insuffisant : 2,2:1 selon abalyseur de contraste des couleurs</t>
+  </si>
+  <si>
+    <t>Avoir un contraste de minimum 3:1 --&gt; choisir des couleurs présentant cette différences de contraste</t>
+  </si>
+  <si>
+    <t>Le site n'est pas responsive</t>
+  </si>
+  <si>
+    <t>Le site n'est pas mobile first, ce qui peut poser un problème pour son SEO, en effet, depuis 2015, google favorise les sites qui sont mobile-first au niveau SEO</t>
+  </si>
+  <si>
+    <t>Absence d'indication de structuration niveau accessibilité c'est-à-dire de balise aria de rôle pour ces éléments de structure</t>
+  </si>
+  <si>
+    <t>Il faut adapter le site en responsive</t>
+  </si>
+  <si>
+    <t>Bouton ne possède pas d'éléments d'accessibilité</t>
+  </si>
+  <si>
+    <t>Quelqu'un qui est malvoyant et utilise une liseuse ne saura en cliquant sur co</t>
+  </si>
+  <si>
+    <t>Quelqu'un qui utilise la tabulation pour avancer dans le site, ne pourra pas percevoir la logique du site et sera un peu déboussoler par l'ordre des éléments qui ne correspond pas au visuel</t>
+  </si>
+  <si>
+    <t>L'ordre du focus ne correspond pas au visuel</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de texte explicatif sur la destination des liens</t>
+  </si>
+  <si>
+    <t>Les gens utilisant par exemple un outil automatiqé de lecture, ne sorront pas le type de lien dont il s'agit</t>
+  </si>
+  <si>
+    <t>Rajouter description du lien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texte écriture avec </t>
+  </si>
+  <si>
+    <t>interlettre (espace entre 2 lettres) pas bon lisibilité (facilité à lire des blocs de texte) pas bonne et longueur de ligne supérieur à 75 caractères</t>
+  </si>
+  <si>
+    <t>citation pas d'utilisation non identifiée structurellement</t>
+  </si>
+  <si>
+    <t>la citation doit maintenant être identifier au niveau duu html</t>
+  </si>
+  <si>
+    <t>A la conception, faire tableau avec ordre de focus et ordre de lecture des éléments</t>
+  </si>
+  <si>
+    <t>identifier la citation à l'aide de la balise &lt;q&gt;  et même blockquote vu la longueur de la citation pas spécialeme,nt besoin d'utiliser un un rôle ARIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,9 +237,16 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +257,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -117,25 +285,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -337,17 +514,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="21.26953125" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="30.36328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.26953125" customWidth="1"/>
     <col min="7" max="26" width="10.54296875" customWidth="1"/>
@@ -357,7 +536,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -393,164 +572,973 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+    <row r="2" spans="1:26" ht="21" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E12" s="4"/>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="31.2">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:26" ht="62.4">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:26" ht="62.4">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="78">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:26" ht="62.4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:26" ht="62.4">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:26" ht="31.2">
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:26" ht="46.8">
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:26" ht="62.4">
+      <c r="B11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" ht="62.4">
+      <c r="B12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E13" s="4"/>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.6">
+      <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:26" ht="17.399999999999999" customHeight="1">
+      <c r="B16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" ht="31.2">
+      <c r="B17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" ht="31.2">
+      <c r="B18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="78">
+      <c r="B21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" ht="31.2">
+      <c r="B23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="93.6">
+      <c r="A24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" ht="46.8">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" ht="62.4">
+      <c r="B26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" ht="78">
+      <c r="A27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B53" s="7"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B55" s="7"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B57" s="7"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B58" s="7"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B59" s="7"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B60" s="7"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B61" s="7"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B62" s="7"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B63" s="7"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B64" s="7"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B65" s="7"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B66" s="7"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B67" s="7"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B68" s="7"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B69" s="7"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B70" s="7"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B71" s="7"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B72" s="7"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+    </row>
+    <row r="73" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B73" s="7"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+    </row>
+    <row r="75" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B75" s="7"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+    </row>
+    <row r="77" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B77" s="7"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+    </row>
+    <row r="78" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+    </row>
+    <row r="79" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B79" s="7"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+    </row>
+    <row r="80" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B80" s="7"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B81" s="7"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+    </row>
+    <row r="82" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B82" s="7"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+    </row>
+    <row r="83" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B83" s="7"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B84" s="7"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+    </row>
+    <row r="85" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B85" s="7"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+    </row>
+    <row r="86" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B86" s="7"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+    </row>
+    <row r="87" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B87" s="7"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+    </row>
+    <row r="88" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B88" s="7"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+    </row>
+    <row r="89" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B89" s="7"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+    </row>
+    <row r="90" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B90" s="7"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+    </row>
+    <row r="91" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B91" s="7"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+    </row>
+    <row r="92" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B92" s="7"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B93" s="7"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+    </row>
+    <row r="94" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B94" s="7"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+    </row>
+    <row r="95" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B95" s="7"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
+    </row>
+    <row r="96" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B96" s="7"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="8"/>
+    </row>
+    <row r="97" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B97" s="7"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="8"/>
+    </row>
+    <row r="98" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B98" s="7"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="8"/>
+    </row>
+    <row r="99" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B99" s="7"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+    </row>
+    <row r="100" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B100" s="7"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+    </row>
+    <row r="101" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B101" s="7"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+    </row>
+    <row r="102" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B102" s="7"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
+    </row>
+    <row r="103" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B103" s="7"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
+    </row>
+    <row r="104" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B104" s="7"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+    </row>
+    <row r="105" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B105" s="7"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8"/>
+    </row>
+    <row r="106" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B106" s="7"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="8"/>
+    </row>
+    <row r="107" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B107" s="7"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+    </row>
+    <row r="108" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B108" s="7"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+    </row>
+    <row r="109" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B109" s="7"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8"/>
+    </row>
+    <row r="110" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B110" s="7"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+    </row>
+    <row r="111" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B111" s="7"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="8"/>
+    </row>
+    <row r="112" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B112" s="7"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="8"/>
+    </row>
+    <row r="113" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B113" s="7"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+    </row>
+    <row r="114" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B114" s="7"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="8"/>
+    </row>
+    <row r="115" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B115" s="7"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
+      <c r="F115" s="8"/>
+    </row>
+    <row r="116" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B116" s="7"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+      <c r="F116" s="8"/>
+    </row>
+    <row r="117" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B117" s="7"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="8"/>
+    </row>
+    <row r="118" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="119" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="120" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="121" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="122" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="123" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="124" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="125" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="126" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="127" spans="2:6" ht="15.75" customHeight="1"/>
+    <row r="128" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="129" ht="15.75" customHeight="1"/>
     <row r="130" ht="15.75" customHeight="1"/>
     <row r="131" ht="15.75" customHeight="1"/>
@@ -1423,8 +2411,9 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modifs fichier audit et modifs et html page principale balise robits et langue
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
   <si>
     <t>Catégorie</t>
   </si>
@@ -38,9 +38,6 @@
     <t>(SEO ou accessiblité ?)</t>
   </si>
   <si>
-    <t>Taille police text centre white</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t xml:space="preserve"> Contraste assez important notamment pour les malvoyants on ne voit pas assez le changement de contraste et donc la possibilité d'interaction</t>
   </si>
   <si>
-    <t>La taille de police est petite c'est une difficulté pour les malvoyants</t>
-  </si>
-  <si>
     <t xml:space="preserve">Côté local de l'agence Lyon </t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>Pas de définition de la langue</t>
   </si>
   <si>
-    <t>Viewport fit cover?</t>
-  </si>
-  <si>
     <t>dans les div bg white te dark, les class sont trop longues</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
     <t>Pas d'indexation des moteurs de recherche</t>
   </si>
   <si>
-    <t>Il faut indiquer via les balises meta name robots qu'on autorise indexation par les moteurs de recherche, sinon il peut y avaoir blocage au niveau des moteurs de recherche</t>
-  </si>
-  <si>
     <t>Pas de balise canonique</t>
   </si>
   <si>
@@ -201,6 +189,87 @@
   </si>
   <si>
     <t>identifier la citation à l'aide de la balise &lt;q&gt;  et même blockquote vu la longueur de la citation pas spécialeme,nt besoin d'utiliser un un rôle ARIA</t>
+  </si>
+  <si>
+    <t>Les liens ne sont pas de qualité</t>
+  </si>
+  <si>
+    <t>ils sont dans le footer, ils ne sont pas de qualité, il n'apportent pas de plus value</t>
+  </si>
+  <si>
+    <t>Faire des liens avec de vrai partenaires qui ne sont pas des concurrents on pourrait mettre un partenaire avec qui on a déjà travaillé et qui a une certaine notoriété</t>
+  </si>
+  <si>
+    <t>Structure/Plan de navigation pas claire</t>
+  </si>
+  <si>
+    <t>Le menu de navigation ne décrit clairement le site ni ce qui se trouve en page 2</t>
+  </si>
+  <si>
+    <t>Phras ed'accroche titre 1 pas assezv catchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le titre 1 ne donne pas d'information sur </t>
+  </si>
+  <si>
+    <t>Taille pde polic inappropriée</t>
+  </si>
+  <si>
+    <t>Augmenter les tailles de police du texte de base</t>
+  </si>
+  <si>
+    <t>Texte h2 pas distingable de l'image de background</t>
+  </si>
+  <si>
+    <t>Faire partie nos réalisations, Faire partie contact, partie notre vision, faire à propos ou présentation, faire partie activités, champ d'activité, champ d'intervention choisi champs d'activité, notre vision, nos réalisations…</t>
+  </si>
+  <si>
+    <t>Balise meta description non complétée</t>
+  </si>
+  <si>
+    <t>renseigner les champs des formulaires avec des indications en exemple</t>
+  </si>
+  <si>
+    <t>Absence de titre page 2 également</t>
+  </si>
+  <si>
+    <t>fournira à google le petit résumé qu'il affiche quand la requête est trouvée</t>
+  </si>
+  <si>
+    <t>accessibilité indications sur le remplissage du formulaire</t>
+  </si>
+  <si>
+    <t>Elle n'est plus lu par google et vient contrarier le principe DRY</t>
+  </si>
+  <si>
+    <t>Présence de balise meta keywords</t>
+  </si>
+  <si>
+    <t>Supprimer la balise</t>
+  </si>
+  <si>
+    <t>Images trop lourdes et trop grandes</t>
+  </si>
+  <si>
+    <t>texte de page non compressé</t>
+  </si>
+  <si>
+    <t>contenu non compressé entraine augmentation du délai de chargement de la page</t>
+  </si>
+  <si>
+    <t>compresser le contenu de la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contenu lourd entraine augmentation du délai de chargement </t>
+  </si>
+  <si>
+    <t>rogner les imgaes pur quelles soient de la taille de leur contenair peu ou prou et compresser les images</t>
+  </si>
+  <si>
+    <t>Il faut indiquer via les balises meta name robots qu'on autorise indexation par les moteurs de recherche, sinon il peut y avoir blocage au niveau des moteurs de recherche</t>
+  </si>
+  <si>
+    <t>&lt;meta name ="robots" content ="index, follow"&gt;</t>
   </si>
 </sst>
 </file>
@@ -246,7 +315,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +331,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,6 +380,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -517,8 +595,8 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
@@ -577,28 +655,28 @@
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="31.2">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -606,13 +684,13 @@
     </row>
     <row r="4" spans="1:26" ht="62.4">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7">
@@ -622,34 +700,34 @@
     </row>
     <row r="5" spans="1:26" ht="62.4">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7">
         <v>2</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="78">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E6" s="7">
         <v>3</v>
@@ -658,39 +736,39 @@
     </row>
     <row r="7" spans="1:26" ht="62.4">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:26" ht="62.4">
       <c r="A8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:26" ht="31.2">
       <c r="B9" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -699,20 +777,20 @@
     </row>
     <row r="10" spans="1:26" ht="46.8">
       <c r="B10" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:26" ht="62.4">
       <c r="B11" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -721,30 +799,28 @@
     </row>
     <row r="12" spans="1:26" ht="62.4">
       <c r="B12" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
-        <v>44</v>
+      <c r="D12" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="B13" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="B14" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -752,7 +828,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.6">
       <c r="B15" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -761,20 +837,20 @@
     </row>
     <row r="16" spans="1:26" ht="17.399999999999999" customHeight="1">
       <c r="B16" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="31.2">
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -783,7 +859,7 @@
     </row>
     <row r="18" spans="1:6" ht="31.2">
       <c r="B18" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -792,7 +868,7 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="B19" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -801,7 +877,7 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="B20" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -810,18 +886,20 @@
     </row>
     <row r="21" spans="1:6" ht="78">
       <c r="B21" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="B22" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -830,10 +908,10 @@
     </row>
     <row r="23" spans="1:6" ht="31.2">
       <c r="B23" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -841,42 +919,42 @@
     </row>
     <row r="24" spans="1:6" ht="93.6">
       <c r="A24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="46.8">
       <c r="A25" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" ht="62.4">
       <c r="B26" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -884,51 +962,76 @@
     </row>
     <row r="27" spans="1:6" ht="78">
       <c r="A27" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+    <row r="28" spans="1:6" ht="93.6">
+      <c r="A28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+    <row r="29" spans="1:6" ht="109.2">
+      <c r="B29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B31" s="7"/>
+    <row r="31" spans="1:6" ht="31.2">
+      <c r="B31" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+    <row r="32" spans="1:6" ht="31.2">
+      <c r="B32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -940,38 +1043,62 @@
       <c r="E33" s="7"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+    <row r="34" spans="2:6" ht="31.2">
+      <c r="B34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B35" s="7"/>
+      <c r="B35" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+    <row r="36" spans="2:6" ht="31.2">
+      <c r="B36" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+    <row r="37" spans="2:6" ht="46.8">
+      <c r="B37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+    <row r="38" spans="2:6" ht="46.8">
+      <c r="B38" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
     </row>

</xml_diff>

<commit_message>
rajout de balise meta titre
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="624" windowWidth="22128" windowHeight="8436" tabRatio="500"/>
+    <workbookView xWindow="936" yWindow="624" windowWidth="18288" windowHeight="8436" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,6 +637,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -678,7 +684,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,6 +700,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -950,13 +959,13 @@
   <dimension ref="A1:Z986"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" style="11" customWidth="1"/>
     <col min="2" max="2" width="33.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
     <col min="4" max="4" width="29.453125" customWidth="1"/>
@@ -966,7 +975,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1006,7 +1015,7 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1023,663 +1032,663 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="12" customFormat="1" ht="62.4" hidden="1">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:26" s="13" customFormat="1" ht="62.4" hidden="1">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="12">
         <v>2</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="12" customFormat="1" ht="62.4" hidden="1">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:26" s="13" customFormat="1" ht="62.4" hidden="1">
+      <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="12">
         <v>2</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="12" customFormat="1" ht="109.2" hidden="1">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:26" s="13" customFormat="1" ht="109.2" hidden="1">
+      <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="12">
         <v>2</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="12" customFormat="1" ht="46.8" hidden="1">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:26" s="13" customFormat="1" ht="46.8">
+      <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="13" customFormat="1" ht="153">
+      <c r="A7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="13" customFormat="1" ht="124.8">
+      <c r="A8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="13" customFormat="1" ht="78" hidden="1">
+      <c r="A9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="12">
         <v>2</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" s="12" customFormat="1" ht="153">
-      <c r="A7" s="13" t="s">
+      <c r="F9" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="13" customFormat="1" ht="93.6" hidden="1">
+      <c r="A10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="B10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="13" customFormat="1" ht="93.6">
+      <c r="A11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="12">
         <v>1</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="12" customFormat="1" ht="124.8" hidden="1">
-      <c r="A8" s="14" t="s">
+      <c r="F11" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="13" customFormat="1" ht="109.2" hidden="1">
+      <c r="A12" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="13" customFormat="1" ht="109.2" hidden="1">
+      <c r="A13" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="12">
+        <v>3</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="13" customFormat="1" ht="109.2">
+      <c r="A14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="B14" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="13" customFormat="1" ht="78">
+      <c r="A15" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="13" customFormat="1" ht="171.6">
+      <c r="A16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="13" customFormat="1" ht="109.2" hidden="1">
+      <c r="A17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="12">
         <v>2</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="12" customFormat="1" ht="78" hidden="1">
-      <c r="A9" s="14" t="s">
+      <c r="F17" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="13" customFormat="1" ht="31.2">
+      <c r="A18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="11">
+      <c r="B18" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="13" customFormat="1" ht="78">
+      <c r="A19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="16" customFormat="1" ht="78" hidden="1">
+      <c r="A20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="12">
         <v>2</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" s="12" customFormat="1" ht="93.6">
-      <c r="A10" s="13" t="s">
+      <c r="F20" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="16" customFormat="1" ht="62.4" hidden="1">
+      <c r="A21" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="B21" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="12">
+        <v>2</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
+      <c r="A22" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
+      <c r="A23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="12">
+        <v>2</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="13" customFormat="1" ht="93.6">
+      <c r="A24" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
+      <c r="A25" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="12">
+        <v>2</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
+      <c r="A26" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="12">
+        <v>2</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="13" customFormat="1" ht="78" hidden="1">
+      <c r="A27" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="12">
+        <v>2</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="16" customFormat="1" ht="93.6" hidden="1">
+      <c r="A28" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="12">
+        <v>2</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
+      <c r="A29" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="12">
+        <v>2</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="16" customFormat="1" ht="62.4" hidden="1">
+      <c r="A30" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="12">
+        <v>2</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="13" customFormat="1" ht="93.6">
+      <c r="A31" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="12">
+        <v>1</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="13" customFormat="1" ht="46.8" hidden="1">
+      <c r="A32" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="12">
+        <v>2</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="13" customFormat="1" ht="109.2" hidden="1">
+      <c r="A33" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="12">
+        <v>2</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
+      <c r="A34" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="12">
+        <v>2</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="13" customFormat="1" ht="78" hidden="1">
+      <c r="A35" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="12">
         <v>3</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="12" customFormat="1" ht="93.6">
-      <c r="A11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="12" customFormat="1" ht="109.2">
-      <c r="A12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="11">
-        <v>2</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="12" customFormat="1" ht="109.2">
-      <c r="A13" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" s="11">
-        <v>3</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" s="12" customFormat="1" ht="109.2" hidden="1">
-      <c r="A14" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="11">
-        <v>1</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" s="12" customFormat="1" ht="78">
-      <c r="A15" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" s="11">
-        <v>1</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" s="12" customFormat="1" ht="171.6">
-      <c r="A16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="E16" s="11">
-        <v>1</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="12" customFormat="1" ht="109.2">
-      <c r="A17" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="11">
-        <v>2</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" ht="31.2" hidden="1">
-      <c r="A18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="11">
-        <v>1</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="12" customFormat="1" ht="78">
-      <c r="A19" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="11">
-        <v>1</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="15" customFormat="1" ht="78">
-      <c r="A20" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="11">
-        <v>2</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="15" customFormat="1" ht="62.4">
-      <c r="A21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="11">
-        <v>2</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="12" customFormat="1" ht="62.4" hidden="1">
-      <c r="A22" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E22" s="11">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="12" customFormat="1" ht="62.4" hidden="1">
-      <c r="A23" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="11">
-        <v>1</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="12" customFormat="1" ht="93.6">
-      <c r="A24" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="11">
-        <v>1</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="12" customFormat="1" ht="62.4">
-      <c r="A25" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="11">
-        <v>2</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="12" customFormat="1" ht="62.4">
-      <c r="A26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="11">
-        <v>2</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="12" customFormat="1" ht="78" hidden="1">
-      <c r="A27" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="11">
-        <v>2</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="15" customFormat="1" ht="93.6" hidden="1">
-      <c r="A28" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="11">
-        <v>2</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="12" customFormat="1" ht="62.4">
-      <c r="A29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" s="11">
-        <v>2</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="15" customFormat="1" ht="62.4" hidden="1">
-      <c r="A30" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E30" s="11">
-        <v>2</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="12" customFormat="1" ht="93.6">
-      <c r="A31" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="E31" s="11">
-        <v>1</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="12" customFormat="1" ht="46.8" hidden="1">
-      <c r="A32" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="11">
-        <v>2</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="12" customFormat="1" ht="109.2">
-      <c r="A33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="11">
-        <v>2</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="12" customFormat="1" ht="62.4">
-      <c r="A34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="E34" s="11">
-        <v>2</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="12" customFormat="1" ht="78">
-      <c r="A35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" s="11">
-        <v>3</v>
-      </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="12" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1733,7 +1742,7 @@
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -1744,7 +1753,7 @@
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -3058,9 +3067,9 @@
     <row r="986" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A2:F35">
-    <filterColumn colId="0">
+    <filterColumn colId="4">
       <filters>
-        <filter val="SEO"/>
+        <filter val="1"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3093,16 +3102,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="23" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test changement couleur bouton contact
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -626,7 +626,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -642,6 +642,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,7 +690,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,6 +728,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -730,18 +758,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -959,8 +975,8 @@
   <dimension ref="A1:Z986"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
@@ -1048,7 +1064,7 @@
       <c r="E3" s="12">
         <v>2</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="25" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1068,7 +1084,7 @@
       <c r="E4" s="12">
         <v>2</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="25" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1092,40 +1108,40 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="13" customFormat="1" ht="46.8">
+    <row r="6" spans="1:26" s="17" customFormat="1" ht="46.8">
       <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="16">
         <v>1</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" ht="153">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:26" s="17" customFormat="1" ht="153">
+      <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="16">
         <v>1</v>
       </c>
       <c r="F7" s="19" t="s">
@@ -1133,7 +1149,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="13" customFormat="1" ht="124.8">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1153,7 +1169,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" s="13" customFormat="1" ht="78" hidden="1">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1192,23 +1208,23 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="13" customFormat="1" ht="93.6">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:26" s="17" customFormat="1" ht="93.6">
+      <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="16">
         <v>1</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="16" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1253,7 +1269,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" s="13" customFormat="1" ht="109.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1272,43 +1288,43 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="13" customFormat="1" ht="78">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:26" s="17" customFormat="1" ht="78">
+      <c r="A15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="16">
         <v>1</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="13" customFormat="1" ht="171.6">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:26" s="17" customFormat="1" ht="171.6">
+      <c r="A16" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="16">
         <v>1</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="16" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1332,48 +1348,48 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="13" customFormat="1" ht="31.2">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:6" s="17" customFormat="1" ht="31.2">
+      <c r="A18" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="16">
         <v>1</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="13" customFormat="1" ht="78">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:6" s="17" customFormat="1" ht="78">
+      <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="16">
         <v>1</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="16" customFormat="1" ht="78" hidden="1">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:6" s="24" customFormat="1" ht="78" hidden="1">
+      <c r="A20" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -1388,12 +1404,12 @@
       <c r="E20" s="12">
         <v>2</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="16" customFormat="1" ht="62.4" hidden="1">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:6" s="24" customFormat="1" ht="62.4" hidden="1">
+      <c r="A21" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -1452,28 +1468,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="13" customFormat="1" ht="93.6">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:6" s="17" customFormat="1" ht="93.6">
+      <c r="A24" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="16">
         <v>1</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="16" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="12" t="s">
@@ -1493,7 +1509,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -1532,8 +1548,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="16" customFormat="1" ht="93.6" hidden="1">
-      <c r="A28" s="15" t="s">
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="93.6" hidden="1">
+      <c r="A28" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -1553,7 +1569,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -1572,8 +1588,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="16" customFormat="1" ht="62.4" hidden="1">
-      <c r="A30" s="15" t="s">
+    <row r="30" spans="1:6" s="24" customFormat="1" ht="62.4" hidden="1">
+      <c r="A30" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="12" t="s">
@@ -1592,28 +1608,28 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="13" customFormat="1" ht="93.6">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="1:6" s="17" customFormat="1" ht="93.6">
+      <c r="A31" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="16">
         <v>1</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="16" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="13" customFormat="1" ht="46.8" hidden="1">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -1633,7 +1649,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" ht="109.2" hidden="1">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -1653,7 +1669,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" s="13" customFormat="1" ht="62.4" hidden="1">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="12" t="s">
@@ -1673,7 +1689,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" s="13" customFormat="1" ht="78" hidden="1">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="12" t="s">
@@ -3102,16 +3118,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="27" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changements couleurs h1 et h2 page 1 uniquement
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -975,8 +975,8 @@
   <dimension ref="A1:Z986"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
@@ -1148,23 +1148,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="13" customFormat="1" ht="124.8">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:26" s="17" customFormat="1" ht="124.8">
+      <c r="A8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="16">
         <v>1</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="16" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>